<commit_message>
Some changes in schematic, added firmware.
</commit_message>
<xml_diff>
--- a/TotalBOM.xlsx
+++ b/TotalBOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>PCB components</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Image sensor</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/100-New-Original-TSL1401CL-TSL1401-Light-To-Frequency-Light-To-Voltage-Linear-Sensor-Array-400dpi-128/32767324096.html</t>
-  </si>
-  <si>
     <t>MCU</t>
   </si>
   <si>
@@ -121,6 +118,18 @@
   </si>
   <si>
     <t>780nm IR Bandpass filter 8.0*8.0mm</t>
+  </si>
+  <si>
+    <t>RPI-352</t>
+  </si>
+  <si>
+    <t>https://ru.aliexpress.com/item/1PCS-TSL1401CL-TSL1401C-TSL1401-SMD-8/32430435025.html</t>
+  </si>
+  <si>
+    <t>150 mm - perimeter length</t>
+  </si>
+  <si>
+    <t>Rubber belt</t>
   </si>
 </sst>
 </file>
@@ -128,9 +137,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +160,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -184,17 +201,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -203,12 +217,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -512,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,7 +541,7 @@
     <col min="1" max="1" width="6.88671875" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" customWidth="1"/>
     <col min="3" max="3" width="18.77734375" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" style="2" customWidth="1"/>
     <col min="5" max="5" width="34.44140625" customWidth="1"/>
     <col min="6" max="6" width="46.77734375" customWidth="1"/>
   </cols>
@@ -535,7 +553,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E1" t="s">
@@ -546,7 +564,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -555,122 +573,122 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>2.75</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+      <c r="A3" s="11"/>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>4</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="11"/>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="8">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="9">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="11"/>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>0.5</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="10">
+      <c r="A6" s="11"/>
+      <c r="B6" s="9">
         <v>5</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>1.5</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="11"/>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="8">
-        <v>7.2</v>
+      <c r="D7" s="7">
+        <v>7.9</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>20</v>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="11"/>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -678,16 +696,16 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="3">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2">
         <v>2.82</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -695,13 +713,13 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>25</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -709,13 +727,13 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>29</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -723,13 +741,33 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="3">
-        <f>SUM(D2:D13)</f>
-        <v>27.37</v>
+        <v>30</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D15" s="2">
+        <f>SUM(D2:D14)</f>
+        <v>30.57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>